<commit_message>
fix: adicionado função para nao deletar coluna essencial para importação
</commit_message>
<xml_diff>
--- a/non_conciliated_data.xlsx
+++ b/non_conciliated_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -49,55 +49,388 @@
     <t>conciliada</t>
   </si>
   <si>
-    <t>2024-10-23 00:00:00</t>
-  </si>
-  <si>
-    <t>2024-10-25 00:00:00</t>
-  </si>
-  <si>
-    <t>VLR. NF. N. 579  DEUCHER RESTAURANTE EIRELI</t>
-  </si>
-  <si>
-    <t>VLR. NF. N. 581  DEUCHER RESTAURANTE EIRELI</t>
-  </si>
-  <si>
-    <t>N/PGTO. NF. N. 578  DEUCHER RESTAURANTE EIRELI</t>
-  </si>
-  <si>
-    <t>N/PGTO. NF. N. 579  DEUCHER RESTAURANTE EIRELI</t>
-  </si>
-  <si>
-    <t>4974</t>
-  </si>
-  <si>
-    <t>5063</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>2024-11-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-05 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-06 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-07 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-08 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-11 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-12 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-13 00:00:00</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3043178 C-04231 2 ISABELA CHEDE CUNHA</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3037877 C-05736 6 EDUARDO ARANTES SOUZA</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3029318 - B-06245 0 ALINE BENTO RADOMINSKI - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>N/PGTO. D.A. 3047509 B-6245 ALINE BENTO RADOMINSKI</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3031186 C-05760 7 LUIZ FELIPE VILELA FEDALTO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3039686 C-05760 7 LUIZ FELIPE VILELA FEDALTO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3047931 B-05160 ISABELA KLOSS KLUPPEL STRO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>N/PGTO. D.A. 3013976 R-3661 3 JESOMIR UBA FILHO</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3040284 - B-04332-7 ELIANE G DE SOUZA BROMBERG - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2954443 C-01807 1 HELENA REBACK GRAICHEN - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3031062 C-02564-3 GIULIANO MIRO ZILIOTTO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3039573 C-02564 3 GIULIANO MIRO ZILIOTTO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>N/PGTO. D.A. 3042200 S-04812 6 ALICE LOBO INFANTE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3044964 - B-01049-1 ODUVALDO BESSA JUNIOR - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>N/PGTO. D.A. 3024156 C-02092 8 GABRIEL DE SOUZA DREHER</t>
+  </si>
+  <si>
+    <t>N/PGTO. D.A. 3024157 C-2092 8 GABRIEL DE SOUZA DREHER</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3048843 B-05042-3 ONILDA CARNEIRO STUNITZ - DUPLICIDA</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2988448 R-03191-9 EDGARD WEIGERT FILHO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3048078 R-01861-5  IRACEMA BETTEGA - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3048239 - B-00461-8 LETICIA ZETOLA PORTES - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3048996 - B-00483-8 MIRABEL LIMA DE OLIVEIRA - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3043140 - B-01092-5 EDUARDA RATTMANN FRAGOSO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2927232 - B-01291-7 CARLOS EDUARDO VIANNA - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2928577 - B-01631-4 REGINA HELENA BRUNI - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3045815 B-01678-1 VALENTIM CLARET SANTOS GON - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3046122 -  B-03457-4 FABIANE PATRICIA E S G VOLAC - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3047814 - B-04843-5 LARA PATRICIA DE CARVALHO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2943089 - B-05133-8 VALERIA MEDEIROS SANTIAGO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3045818 B-05153-7 LUIS MIGUEL JUSTO DA SILVA - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3048223 B-05777-0 MARCELLE CAVALINI SOARES - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3046136 - B-05777-0 ALICIA CAVALINI SOARES - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2965901 -  B-05915-9 ELISA BEATRIZ DALLEDONE SIQU - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2970798 -  B-06163-4 CARLOS AFONSO CARMEZIM GO - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2954626 - C-01842-1 LETICIA ALLAGE SELEME DE CAM - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3043789 - C-02194-2 RICARDO BISCAIA BACELLAR - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3047559 - C-03339-2  MIKAELA SCHIER KAMINSKI - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2990658 - R-03773-2 WANIA MANTOVANI GUTIERREZ - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2980516 - S-00642-1 SARAH CARBONAR DE OLIVEIRA - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3022028 -  S-04812-6 ALICE LOBO INFANTE DA C TEIXE - DUPLICIDADE</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 2926931 B-01217 3 ANNA BEATRIZ DE LACERDA PIN</t>
+  </si>
+  <si>
+    <t>VLR. REC. MENSALIDADES/OUTROS BRADESCO D.A. 3047541 - S00313 2 VICTORIA SOARES SIMAS</t>
+  </si>
+  <si>
+    <t>5073</t>
+  </si>
+  <si>
+    <t>5075</t>
+  </si>
+  <si>
+    <t>5079</t>
+  </si>
+  <si>
+    <t>5149</t>
+  </si>
+  <si>
+    <t>5166</t>
+  </si>
+  <si>
+    <t>5193</t>
+  </si>
+  <si>
+    <t>5233</t>
+  </si>
+  <si>
+    <t>5195</t>
+  </si>
+  <si>
+    <t>5235</t>
+  </si>
+  <si>
+    <t>5241</t>
+  </si>
+  <si>
+    <t>5242</t>
+  </si>
+  <si>
+    <t>5249</t>
+  </si>
+  <si>
+    <t>5257</t>
+  </si>
+  <si>
+    <t>5258</t>
+  </si>
+  <si>
+    <t>5276</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>51</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>52</t>
   </si>
   <si>
     <t>53</t>
   </si>
   <si>
-    <t>81640</t>
-  </si>
-  <si>
-    <t>6540</t>
-  </si>
-  <si>
-    <t>6960</t>
+    <t>28</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>184.62</t>
+  </si>
+  <si>
+    <t>363.24</t>
+  </si>
+  <si>
+    <t>285.6</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>182.7</t>
+  </si>
+  <si>
+    <t>136.84</t>
+  </si>
+  <si>
+    <t>135.64</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>164.55</t>
+  </si>
+  <si>
+    <t>734.76</t>
+  </si>
+  <si>
+    <t>205.95</t>
+  </si>
+  <si>
+    <t>203.85</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>595</t>
+  </si>
+  <si>
+    <t>371.22</t>
+  </si>
+  <si>
+    <t>170.7</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>76.83</t>
+  </si>
+  <si>
+    <t>714</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1095</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t>736.2</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>02089</t>
+    <t>04426</t>
   </si>
 </sst>
 </file>
@@ -455,7 +788,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,28 +831,28 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -527,28 +860,28 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -556,28 +889,28 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -585,30 +918,1103 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" t="s">
+        <v>138</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" t="s">
+        <v>138</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J12" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" t="s">
+        <v>138</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" t="s">
+        <v>137</v>
+      </c>
+      <c r="J18" t="s">
+        <v>138</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" t="s">
+        <v>138</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" t="s">
+        <v>138</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J22" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" t="s">
+        <v>138</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" t="s">
+        <v>131</v>
+      </c>
+      <c r="I24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" t="s">
+        <v>138</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" t="s">
+        <v>132</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26" t="s">
+        <v>138</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="J5" t="s">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" t="s">
+        <v>138</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="K5">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" t="s">
+        <v>133</v>
+      </c>
+      <c r="I28" t="s">
+        <v>137</v>
+      </c>
+      <c r="J28" t="s">
+        <v>138</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" t="s">
+        <v>138</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I30" t="s">
+        <v>137</v>
+      </c>
+      <c r="J30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" t="s">
+        <v>137</v>
+      </c>
+      <c r="J31" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" t="s">
+        <v>137</v>
+      </c>
+      <c r="J32" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" t="s">
+        <v>137</v>
+      </c>
+      <c r="J33" t="s">
+        <v>138</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" t="s">
+        <v>137</v>
+      </c>
+      <c r="J34" t="s">
+        <v>138</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35" t="s">
+        <v>137</v>
+      </c>
+      <c r="J35" t="s">
+        <v>138</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" t="s">
+        <v>138</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="H37" t="s">
+        <v>131</v>
+      </c>
+      <c r="I37" t="s">
+        <v>137</v>
+      </c>
+      <c r="J37" t="s">
+        <v>138</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" t="s">
+        <v>106</v>
+      </c>
+      <c r="H38" t="s">
+        <v>135</v>
+      </c>
+      <c r="I38" t="s">
+        <v>137</v>
+      </c>
+      <c r="J38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
+        <v>107</v>
+      </c>
+      <c r="H39" t="s">
+        <v>135</v>
+      </c>
+      <c r="I39" t="s">
+        <v>137</v>
+      </c>
+      <c r="J39" t="s">
+        <v>138</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" t="s">
+        <v>137</v>
+      </c>
+      <c r="J40" t="s">
+        <v>138</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" t="s">
+        <v>136</v>
+      </c>
+      <c r="I41" t="s">
+        <v>137</v>
+      </c>
+      <c r="J41" t="s">
+        <v>138</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" t="s">
+        <v>86</v>
+      </c>
+      <c r="H42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" t="s">
+        <v>137</v>
+      </c>
+      <c r="J42" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42">
         <v>0</v>
       </c>
     </row>

</xml_diff>